<commit_message>
Lots of fix and improvement
</commit_message>
<xml_diff>
--- a/report_template/calibration_monthly.xlsx
+++ b/report_template/calibration_monthly.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="校正月報" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>校正月報表</t>
   </si>
@@ -92,15 +92,25 @@
   <si>
     <t>全幅法規_x000D_
 偏移率(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">大城站(甲烷)   全幅校正趨勢圖
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">大城站(甲烷)   零點校正趨勢圖
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -193,7 +203,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -221,14 +231,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -248,7 +261,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
@@ -263,52 +276,31 @@
   <c:chart>
     <c:title>
       <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="zh-TW" altLang="en-US" sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>大城站</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-TW" sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>(</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="zh-TW" altLang="en-US" sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>甲烷</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-TW" sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>)   </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="zh-TW" altLang="en-US" sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>零點校正趨勢圖</a:t>
-            </a:r>
-            <a:endParaRPr altLang="en-US" sz="1600">
+        <c:strRef>
+          <c:f>校正月報!$A$37</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>大城站(甲烷)   零點校正趨勢圖
+</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600">
               <a:latin typeface="Arial"/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -341,6 +333,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE67-46B7-80F3-7E92C29BC138}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -378,6 +375,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CE67-46B7-80F3-7E92C29BC138}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -414,6 +416,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CE67-46B7-80F3-7E92C29BC138}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -448,10 +455,10 @@
                   <a:rPr lang="zh-TW" altLang="en-US"/>
                   <a:t>日期</a:t>
                 </a:r>
-                <a:endParaRPr altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -485,10 +492,10 @@
                   <a:rPr lang="zh-TW" altLang="en-US"/>
                   <a:t>監測值</a:t>
                 </a:r>
-                <a:endParaRPr altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00_ " sourceLinked="1"/>
@@ -502,6 +509,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -517,7 +525,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
@@ -532,52 +540,30 @@
   <c:chart>
     <c:title>
       <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="zh-TW" altLang="en-US" sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>大城站</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-TW" sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>(</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="zh-TW" altLang="en-US" sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>甲烷</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-TW" sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>)   </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="zh-TW" altLang="en-US" sz="1600">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>全幅校正趨勢圖</a:t>
-            </a:r>
-            <a:endParaRPr altLang="en-US" sz="1600">
-              <a:latin typeface="Arial"/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
+        <c:strRef>
+          <c:f>校正月報!$A$38</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>大城站(甲烷)   全幅校正趨勢圖
+</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
       </c:tx>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -610,6 +596,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-37D1-4BDD-ABEE-A7984354487A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -647,6 +638,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-37D1-4BDD-ABEE-A7984354487A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -683,6 +679,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-37D1-4BDD-ABEE-A7984354487A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -717,7 +718,6 @@
                   <a:rPr lang="zh-TW" altLang="en-US"/>
                   <a:t>日期</a:t>
                 </a:r>
-                <a:endParaRPr altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -754,7 +754,6 @@
                   <a:rPr lang="zh-TW" altLang="en-US"/>
                   <a:t>監測值</a:t>
                 </a:r>
-                <a:endParaRPr altLang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1137,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1149,52 +1148,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="10"/>
+      <c r="M2" s="12"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
       <c r="I3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1202,10 +1201,10 @@
         <v>16</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="10"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1253,16 +1252,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
       <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1270,16 +1269,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1287,16 +1286,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1304,16 +1303,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
       <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1321,16 +1320,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1338,16 +1337,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1355,16 +1354,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
       <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1372,16 +1371,16 @@
         <v>8</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1389,16 +1388,16 @@
         <v>9</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
       <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1406,16 +1405,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
       <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1423,16 +1422,16 @@
         <v>11</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
       <c r="M15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1440,16 +1439,16 @@
         <v>12</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
       <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1457,16 +1456,16 @@
         <v>13</v>
       </c>
       <c r="B17" s="7"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1474,16 +1473,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="7"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1491,16 +1490,16 @@
         <v>15</v>
       </c>
       <c r="B19" s="7"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
       <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1508,16 +1507,16 @@
         <v>16</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
       <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1525,16 +1524,16 @@
         <v>17</v>
       </c>
       <c r="B21" s="7"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
       <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1542,16 +1541,16 @@
         <v>18</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
       <c r="M22" s="8"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1559,16 +1558,16 @@
         <v>19</v>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1576,16 +1575,16 @@
         <v>20</v>
       </c>
       <c r="B24" s="7"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
       <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1593,16 +1592,16 @@
         <v>21</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
       <c r="M25" s="8"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1610,16 +1609,16 @@
         <v>22</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
       <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1627,16 +1626,16 @@
         <v>23</v>
       </c>
       <c r="B27" s="8"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
       <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1644,16 +1643,16 @@
         <v>24</v>
       </c>
       <c r="B28" s="8"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
       <c r="M28" s="8"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1661,16 +1660,16 @@
         <v>25</v>
       </c>
       <c r="B29" s="8"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
       <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1678,16 +1677,16 @@
         <v>26</v>
       </c>
       <c r="B30" s="8"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1695,16 +1694,16 @@
         <v>27</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1712,16 +1711,16 @@
         <v>28</v>
       </c>
       <c r="B32" s="8"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
       <c r="M32" s="8"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -1729,16 +1728,16 @@
         <v>29</v>
       </c>
       <c r="B33" s="8"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
       <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -1746,16 +1745,16 @@
         <v>30</v>
       </c>
       <c r="B34" s="8"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
       <c r="M34" s="8"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -1763,20 +1762,38 @@
         <v>31</v>
       </c>
       <c r="B35" s="8"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
       <c r="M35" s="8"/>
     </row>
+    <row r="37" spans="1:13" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" spans="1:13" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:D38"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="L2:M2"/>

</xml_diff>